<commit_message>
Commit number 13(remote to Github) Rejects
</commit_message>
<xml_diff>
--- a/src/main/java/selenium_core/excel_sheets_data/selenium_test_data.xlsx
+++ b/src/main/java/selenium_core/excel_sheets_data/selenium_test_data.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stanislav/IdeaProjects/selnium_core_full_automation/src/main/java/selenium_core/excel_sheets_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{4E6DCEC2-5026-8147-8339-7578C11C34FA}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D17B62-9E13-4F45-9A2A-179098093959}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="16240" windowWidth="28800" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="data" r:id="rId1" sheetId="1"/>
-    <sheet name="TestControl" r:id="rId2" sheetId="2"/>
-    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginData" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Test</t>
   </si>
@@ -90,30 +90,32 @@
     <t>wait</t>
   </si>
   <si>
-    <t>TestSkript</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Signin</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>FAILED</t>
-  </si>
-  <si>
-    <t>SKIP</t>
+    <t>StartLoginTest</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Pasword</t>
+  </si>
+  <si>
+    <t>123456789@</t>
+  </si>
+  <si>
+    <t>RanMode</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>stasman9@mail.ru</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,8 +144,21 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,6 +180,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -219,50 +252,69 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="0">
+  <cellStyleXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="1" applyFont="1" borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="4" fontId="4" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="3" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle builtinId="9" hidden="1" name="Followed Hyperlink" xfId="2"/>
-    <cellStyle builtinId="8" hidden="1" name="Hyperlink" xfId="1"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  <cellStyles count="4">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -279,10 +331,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -317,7 +369,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="맑은 고딕"/>
+        <a:latin typeface="맑은 고딕" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -352,7 +404,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="맑은 고딕"/>
+        <a:latin typeface="맑은 고딕" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -446,21 +498,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -477,7 +529,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -529,17 +581,17 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="200">
+    <sheetView zoomScale="200" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -645,62 +697,91 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="135">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row ht="16" r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+      <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row ht="16" r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+      <c r="A2" s="12"/>
+      <c r="B2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row ht="16" r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row ht="16" r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D2" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+      <c r="A3" s="12"/>
+      <c r="B3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+      <c r="A4" s="12"/>
+      <c r="B4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{AE91C608-FA91-1C48-8AFB-EE77FC5CD2C5}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{7CED4F2B-60EC-4444-9367-5F5CAADE36B6}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{0C42A2B0-A53B-D64B-B04B-CAFED7FDDA4C}"/>
+    <hyperlink ref="B4" r:id="rId4" xr:uid="{89C083F6-E926-4945-B4A4-ACB2A0DBCBCE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -708,7 +789,7 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>